<commit_message>
Transportation file updates from CB
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -1,28 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\AVL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\Current CA EPS update\Transportation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1CE54D-E936-4E1D-BF70-14E5056F61E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="23955" windowHeight="13545"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
     <sheet name="NTS 1-20" sheetId="11" r:id="rId2"/>
     <sheet name="Data" sheetId="2" r:id="rId3"/>
-    <sheet name="AVL" sheetId="10" r:id="rId4"/>
+    <sheet name="ARB freight" sheetId="12" r:id="rId4"/>
+    <sheet name="AVL" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
   <si>
     <t>Car Avg Lifetime, years (Page 22, Table 7)</t>
   </si>
@@ -355,11 +369,20 @@
   <si>
     <t>Vehicle Lifetime (years)</t>
   </si>
+  <si>
+    <t xml:space="preserve">CARB states limit on truck life is 25 years. </t>
+  </si>
+  <si>
+    <t>Limit to 25 years based on below.</t>
+  </si>
+  <si>
+    <t>https://ww2.arb.ca.gov/sites/default/files/2018-12/181204workgrouppresentation.pdf</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="###0.00_)"/>
     <numFmt numFmtId="165" formatCode="\(\R\)General"/>
@@ -1460,9 +1483,24 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1471,21 +1509,6 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="27" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="22" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="15" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -1514,41 +1537,41 @@
     <cellStyle name="Accent5" xfId="50" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="54" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="23" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Body: normal cell" xfId="3"/>
+    <cellStyle name="Body: normal cell" xfId="3" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
     <cellStyle name="Calculation" xfId="27" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="29" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Data" xfId="14"/>
-    <cellStyle name="Data no deci" xfId="61"/>
+    <cellStyle name="Data" xfId="14" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Data no deci" xfId="61" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
     <cellStyle name="Explanatory Text" xfId="32" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="9"/>
-    <cellStyle name="Footnotes: all except top row" xfId="12"/>
-    <cellStyle name="Footnotes: top row" xfId="7"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="9" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="12" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="7" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
     <cellStyle name="Good" xfId="22" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Header: bottom row" xfId="2"/>
-    <cellStyle name="Header: top rows" xfId="4"/>
+    <cellStyle name="Header: bottom row" xfId="2" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="Header: top rows" xfId="4" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
     <cellStyle name="Heading 1" xfId="18" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="19" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="20" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="21" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hed Side" xfId="15"/>
-    <cellStyle name="Hed Side Regular" xfId="60"/>
-    <cellStyle name="Hed Top" xfId="59"/>
+    <cellStyle name="Hed Side" xfId="15" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="Hed Side Regular" xfId="60" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="Hed Top" xfId="59" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="10"/>
+    <cellStyle name="Hyperlink 2" xfId="10" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
     <cellStyle name="Input" xfId="25" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="28" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="24" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="31" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="26" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
     <cellStyle name="Percent" xfId="16" builtinId="5"/>
-    <cellStyle name="Section Break" xfId="8"/>
-    <cellStyle name="Section Break: parent row" xfId="5"/>
-    <cellStyle name="Table title" xfId="13"/>
+    <cellStyle name="Section Break" xfId="8" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Section Break: parent row" xfId="5" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Table title" xfId="13" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
     <cellStyle name="Title" xfId="17" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Title-2" xfId="58"/>
+    <cellStyle name="Title-2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
     <cellStyle name="Total" xfId="33" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="30" builtinId="11" customBuiltin="1"/>
   </cellStyles>
@@ -1579,7 +1602,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="2">
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1593,6 +1616,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>42863</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>95308</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47653</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B5719C9-1915-4CFD-BD00-CDB395E2C23C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2068513"/>
+          <a:ext cx="7410508" cy="3871940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1671,6 +1743,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1706,6 +1795,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1881,22 +1987,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="132.265625" customWidth="1"/>
+    <col min="2" max="2" width="132.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
@@ -1904,325 +2012,326 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="10">
         <v>2006</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" s="9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="10">
         <v>2016</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="10">
         <v>2015</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="9" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B26" s="10">
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="9" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B32" s="10">
         <v>2013</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" s="20">
         <v>2009</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="25" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B49" s="13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>99</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B41" r:id="rId2"/>
-    <hyperlink ref="B48" r:id="rId3"/>
-    <hyperlink ref="B28" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B41" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B48" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B21" r:id="rId5" xr:uid="{6E116428-2E91-4C31-B303-F961C6760DF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BC61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:AB1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" style="13" customWidth="1"/>
-    <col min="2" max="27" width="7.73046875" style="13" customWidth="1"/>
-    <col min="28" max="28" width="7.1328125" style="77" customWidth="1"/>
-    <col min="29" max="55" width="9.1328125" style="77"/>
-    <col min="56" max="16384" width="9.1328125" style="13"/>
+    <col min="1" max="1" width="19.36328125" style="13" customWidth="1"/>
+    <col min="2" max="27" width="7.7265625" style="13" customWidth="1"/>
+    <col min="28" max="28" width="7.08984375" style="77" customWidth="1"/>
+    <col min="29" max="55" width="9.08984375" style="77"/>
+    <col min="56" max="16384" width="9.08984375" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="91" t="s">
+    <row r="1" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
-      <c r="J1" s="91"/>
-      <c r="K1" s="91"/>
-      <c r="L1" s="91"/>
-      <c r="M1" s="91"/>
-      <c r="N1" s="91"/>
-      <c r="O1" s="91"/>
-      <c r="P1" s="91"/>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
-      <c r="S1" s="91"/>
-      <c r="T1" s="91"/>
-      <c r="U1" s="91"/>
-      <c r="V1" s="91"/>
-      <c r="W1" s="91"/>
-      <c r="X1" s="91"/>
-      <c r="Y1" s="91"/>
-      <c r="Z1" s="91"/>
-      <c r="AA1" s="91"/>
-      <c r="AB1" s="91"/>
-      <c r="AC1" s="92"/>
-      <c r="AD1" s="92"/>
-      <c r="AE1" s="92"/>
-      <c r="AF1" s="92"/>
-      <c r="AG1" s="92"/>
-      <c r="AH1" s="92"/>
-      <c r="AI1" s="92"/>
-      <c r="AJ1" s="92"/>
-      <c r="AK1" s="92"/>
-      <c r="AL1" s="92"/>
-      <c r="AM1" s="92"/>
-      <c r="AN1" s="92"/>
-      <c r="AO1" s="92"/>
-      <c r="AP1" s="92"/>
-      <c r="AQ1" s="92"/>
-      <c r="AR1" s="92"/>
-      <c r="AS1" s="92"/>
-      <c r="AT1" s="92"/>
-      <c r="AU1" s="92"/>
-      <c r="AV1" s="92"/>
-      <c r="AW1" s="92"/>
-      <c r="AX1" s="92"/>
-      <c r="AY1" s="92"/>
-      <c r="AZ1" s="92"/>
-      <c r="BA1" s="92"/>
-      <c r="BB1" s="92"/>
-    </row>
-    <row r="2" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
+      <c r="I1" s="89"/>
+      <c r="J1" s="89"/>
+      <c r="K1" s="89"/>
+      <c r="L1" s="89"/>
+      <c r="M1" s="89"/>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
+      <c r="P1" s="89"/>
+      <c r="Q1" s="89"/>
+      <c r="R1" s="89"/>
+      <c r="S1" s="89"/>
+      <c r="T1" s="89"/>
+      <c r="U1" s="89"/>
+      <c r="V1" s="89"/>
+      <c r="W1" s="89"/>
+      <c r="X1" s="89"/>
+      <c r="Y1" s="89"/>
+      <c r="Z1" s="89"/>
+      <c r="AA1" s="89"/>
+      <c r="AB1" s="89"/>
+      <c r="AC1" s="90"/>
+      <c r="AD1" s="90"/>
+      <c r="AE1" s="90"/>
+      <c r="AF1" s="90"/>
+      <c r="AG1" s="90"/>
+      <c r="AH1" s="90"/>
+      <c r="AI1" s="90"/>
+      <c r="AJ1" s="90"/>
+      <c r="AK1" s="90"/>
+      <c r="AL1" s="90"/>
+      <c r="AM1" s="90"/>
+      <c r="AN1" s="90"/>
+      <c r="AO1" s="90"/>
+      <c r="AP1" s="90"/>
+      <c r="AQ1" s="90"/>
+      <c r="AR1" s="90"/>
+      <c r="AS1" s="90"/>
+      <c r="AT1" s="90"/>
+      <c r="AU1" s="90"/>
+      <c r="AV1" s="90"/>
+      <c r="AW1" s="90"/>
+      <c r="AX1" s="90"/>
+      <c r="AY1" s="90"/>
+      <c r="AZ1" s="90"/>
+      <c r="BA1" s="90"/>
+      <c r="BB1" s="90"/>
+    </row>
+    <row r="2" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="46"/>
       <c r="B2" s="47">
         <v>1980</v>
@@ -2332,7 +2441,7 @@
       <c r="BA2" s="53"/>
       <c r="BB2" s="54"/>
     </row>
-    <row r="3" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="55" t="s">
         <v>65</v>
       </c>
@@ -2444,7 +2553,7 @@
       <c r="BA3" s="58"/>
       <c r="BB3" s="58"/>
     </row>
-    <row r="4" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="59" t="s">
         <v>67</v>
       </c>
@@ -2556,7 +2665,7 @@
       <c r="BA4" s="63"/>
       <c r="BB4" s="63"/>
     </row>
-    <row r="5" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
         <v>68</v>
       </c>
@@ -2668,7 +2777,7 @@
       <c r="BA5" s="63"/>
       <c r="BB5" s="63"/>
     </row>
-    <row r="6" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="59" t="s">
         <v>69</v>
       </c>
@@ -2780,7 +2889,7 @@
       <c r="BA6" s="63"/>
       <c r="BB6" s="63"/>
     </row>
-    <row r="7" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="59" t="s">
         <v>70</v>
       </c>
@@ -2892,7 +3001,7 @@
       <c r="BA7" s="63"/>
       <c r="BB7" s="63"/>
     </row>
-    <row r="8" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
         <v>71</v>
       </c>
@@ -3004,7 +3113,7 @@
       <c r="BA8" s="63"/>
       <c r="BB8" s="63"/>
     </row>
-    <row r="9" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="64" t="s">
         <v>72</v>
       </c>
@@ -3062,7 +3171,7 @@
       <c r="BA9" s="66"/>
       <c r="BB9" s="66"/>
     </row>
-    <row r="10" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59" t="s">
         <v>67</v>
       </c>
@@ -3176,7 +3285,7 @@
       <c r="BA10" s="68"/>
       <c r="BB10" s="68"/>
     </row>
-    <row r="11" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59" t="s">
         <v>68</v>
       </c>
@@ -3288,7 +3397,7 @@
       <c r="BA11" s="68"/>
       <c r="BB11" s="68"/>
     </row>
-    <row r="12" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="59" t="s">
         <v>69</v>
       </c>
@@ -3400,7 +3509,7 @@
       <c r="BA12" s="68"/>
       <c r="BB12" s="68"/>
     </row>
-    <row r="13" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59" t="s">
         <v>70</v>
       </c>
@@ -3512,7 +3621,7 @@
       <c r="BA13" s="68"/>
       <c r="BB13" s="68"/>
     </row>
-    <row r="14" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59" t="s">
         <v>71</v>
       </c>
@@ -3624,7 +3733,7 @@
       <c r="BA14" s="68"/>
       <c r="BB14" s="68"/>
     </row>
-    <row r="15" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="55" t="s">
         <v>73</v>
       </c>
@@ -3682,7 +3791,7 @@
       <c r="BA15" s="70"/>
       <c r="BB15" s="70"/>
     </row>
-    <row r="16" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="59" t="s">
         <v>67</v>
       </c>
@@ -3794,7 +3903,7 @@
       <c r="BA16" s="72"/>
       <c r="BB16" s="72"/>
     </row>
-    <row r="17" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="59" t="s">
         <v>68</v>
       </c>
@@ -3906,7 +4015,7 @@
       <c r="BA17" s="72"/>
       <c r="BB17" s="72"/>
     </row>
-    <row r="18" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="59" t="s">
         <v>69</v>
       </c>
@@ -4018,7 +4127,7 @@
       <c r="BA18" s="72"/>
       <c r="BB18" s="72"/>
     </row>
-    <row r="19" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="59" t="s">
         <v>70</v>
       </c>
@@ -4130,7 +4239,7 @@
       <c r="BA19" s="72"/>
       <c r="BB19" s="72"/>
     </row>
-    <row r="20" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="73" t="s">
         <v>71</v>
       </c>
@@ -4242,258 +4351,260 @@
       <c r="BA20" s="72"/>
       <c r="BB20" s="72"/>
     </row>
-    <row r="21" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="93" t="s">
+    <row r="21" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="91" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="93"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="93"/>
-      <c r="G21" s="93"/>
-      <c r="H21" s="93"/>
-      <c r="I21" s="93"/>
-      <c r="J21" s="93"/>
-      <c r="K21" s="93"/>
-      <c r="L21" s="93"/>
-      <c r="M21" s="93"/>
-      <c r="N21" s="93"/>
-      <c r="O21" s="93"/>
-      <c r="P21" s="93"/>
-      <c r="Q21" s="93"/>
-    </row>
-    <row r="22" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="94"/>
-      <c r="B22" s="94"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="94"/>
-      <c r="I22" s="94"/>
-      <c r="J22" s="94"/>
-      <c r="K22" s="94"/>
-      <c r="L22" s="94"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="94"/>
-      <c r="O22" s="94"/>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="94"/>
-    </row>
-    <row r="23" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="94" t="s">
+      <c r="B21" s="91"/>
+      <c r="C21" s="91"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="91"/>
+      <c r="F21" s="91"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
+      <c r="J21" s="91"/>
+      <c r="K21" s="91"/>
+      <c r="L21" s="91"/>
+      <c r="M21" s="91"/>
+      <c r="N21" s="91"/>
+      <c r="O21" s="91"/>
+      <c r="P21" s="91"/>
+      <c r="Q21" s="91"/>
+    </row>
+    <row r="22" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="92"/>
+      <c r="B22" s="92"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
+      <c r="F22" s="92"/>
+      <c r="G22" s="92"/>
+      <c r="H22" s="92"/>
+      <c r="I22" s="92"/>
+      <c r="J22" s="92"/>
+      <c r="K22" s="92"/>
+      <c r="L22" s="92"/>
+      <c r="M22" s="92"/>
+      <c r="N22" s="92"/>
+      <c r="O22" s="92"/>
+      <c r="P22" s="92"/>
+      <c r="Q22" s="92"/>
+    </row>
+    <row r="23" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
-      <c r="D23" s="94"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="94"/>
-      <c r="J23" s="94"/>
-      <c r="K23" s="94"/>
-      <c r="L23" s="94"/>
-      <c r="M23" s="94"/>
-      <c r="N23" s="94"/>
-      <c r="O23" s="94"/>
-      <c r="P23" s="94"/>
-      <c r="Q23" s="94"/>
-    </row>
-    <row r="24" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="87" t="s">
+      <c r="B23" s="92"/>
+      <c r="C23" s="92"/>
+      <c r="D23" s="92"/>
+      <c r="E23" s="92"/>
+      <c r="F23" s="92"/>
+      <c r="G23" s="92"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="92"/>
+      <c r="J23" s="92"/>
+      <c r="K23" s="92"/>
+      <c r="L23" s="92"/>
+      <c r="M23" s="92"/>
+      <c r="N23" s="92"/>
+      <c r="O23" s="92"/>
+      <c r="P23" s="92"/>
+      <c r="Q23" s="92"/>
+    </row>
+    <row r="24" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="88" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="87"/>
-      <c r="C24" s="87"/>
-      <c r="D24" s="87"/>
-      <c r="E24" s="87"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="87"/>
-      <c r="H24" s="87"/>
-      <c r="I24" s="87"/>
-      <c r="J24" s="87"/>
-      <c r="K24" s="87"/>
-      <c r="L24" s="87"/>
-      <c r="M24" s="87"/>
-      <c r="N24" s="87"/>
-      <c r="O24" s="87"/>
-      <c r="P24" s="87"/>
-      <c r="Q24" s="87"/>
-    </row>
-    <row r="25" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="87" t="s">
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="88"/>
+      <c r="P24" s="88"/>
+      <c r="Q24" s="88"/>
+    </row>
+    <row r="25" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="87"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="87"/>
-      <c r="J25" s="87"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="87"/>
-      <c r="M25" s="87"/>
-      <c r="N25" s="87"/>
-      <c r="O25" s="87"/>
-      <c r="P25" s="87"/>
-      <c r="Q25" s="87"/>
-    </row>
-    <row r="26" spans="1:54" s="76" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="88" t="s">
+      <c r="B25" s="88"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="88"/>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
+      <c r="K25" s="88"/>
+      <c r="L25" s="88"/>
+      <c r="M25" s="88"/>
+      <c r="N25" s="88"/>
+      <c r="O25" s="88"/>
+      <c r="P25" s="88"/>
+      <c r="Q25" s="88"/>
+    </row>
+    <row r="26" spans="1:54" s="76" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="88"/>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
-    </row>
-    <row r="27" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="88"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="88"/>
-      <c r="D27" s="88"/>
-      <c r="E27" s="88"/>
-      <c r="F27" s="88"/>
-      <c r="G27" s="88"/>
-      <c r="H27" s="88"/>
-      <c r="I27" s="88"/>
-      <c r="J27" s="88"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="88"/>
-      <c r="M27" s="88"/>
-      <c r="N27" s="88"/>
-      <c r="O27" s="88"/>
-      <c r="P27" s="88"/>
-      <c r="Q27" s="88"/>
-    </row>
-    <row r="28" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="89" t="s">
+      <c r="B26" s="93"/>
+      <c r="C26" s="93"/>
+      <c r="D26" s="93"/>
+      <c r="E26" s="93"/>
+      <c r="F26" s="93"/>
+      <c r="G26" s="93"/>
+      <c r="H26" s="93"/>
+      <c r="I26" s="93"/>
+      <c r="J26" s="93"/>
+      <c r="K26" s="93"/>
+      <c r="L26" s="93"/>
+      <c r="M26" s="93"/>
+      <c r="N26" s="93"/>
+      <c r="O26" s="93"/>
+      <c r="P26" s="93"/>
+      <c r="Q26" s="93"/>
+    </row>
+    <row r="27" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="93"/>
+      <c r="B27" s="93"/>
+      <c r="C27" s="93"/>
+      <c r="D27" s="93"/>
+      <c r="E27" s="93"/>
+      <c r="F27" s="93"/>
+      <c r="G27" s="93"/>
+      <c r="H27" s="93"/>
+      <c r="I27" s="93"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="93"/>
+      <c r="L27" s="93"/>
+      <c r="M27" s="93"/>
+      <c r="N27" s="93"/>
+      <c r="O27" s="93"/>
+      <c r="P27" s="93"/>
+      <c r="Q27" s="93"/>
+    </row>
+    <row r="28" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="94" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="89"/>
-      <c r="C28" s="89"/>
-      <c r="D28" s="89"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="89"/>
-      <c r="G28" s="89"/>
-      <c r="H28" s="89"/>
-      <c r="I28" s="89"/>
-      <c r="J28" s="89"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="89"/>
-      <c r="M28" s="89"/>
-      <c r="N28" s="89"/>
-      <c r="O28" s="89"/>
-      <c r="P28" s="89"/>
-      <c r="Q28" s="89"/>
-    </row>
-    <row r="29" spans="1:54" s="76" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="90" t="s">
+      <c r="B28" s="94"/>
+      <c r="C28" s="94"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="94"/>
+      <c r="M28" s="94"/>
+      <c r="N28" s="94"/>
+      <c r="O28" s="94"/>
+      <c r="P28" s="94"/>
+      <c r="Q28" s="94"/>
+    </row>
+    <row r="29" spans="1:54" s="76" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="90"/>
-      <c r="C29" s="90"/>
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="90"/>
-      <c r="G29" s="90"/>
-      <c r="H29" s="90"/>
-      <c r="I29" s="90"/>
-      <c r="J29" s="90"/>
-      <c r="K29" s="90"/>
-      <c r="L29" s="90"/>
-      <c r="M29" s="90"/>
-      <c r="N29" s="90"/>
-      <c r="O29" s="90"/>
-      <c r="P29" s="90"/>
-      <c r="Q29" s="90"/>
-    </row>
-    <row r="30" spans="1:54" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="31" spans="1:54" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="1:54" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="33" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="34" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="35" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="36" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="37" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="38" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="39" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="40" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="41" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="42" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="43" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="44" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="45" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="46" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="47" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="48" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="49" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="50" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="51" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="52" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="53" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="54" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="55" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="56" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="57" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="58" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="59" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="60" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="61" s="77" customFormat="1" x14ac:dyDescent="0.45"/>
+      <c r="B29" s="95"/>
+      <c r="C29" s="95"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="95"/>
+      <c r="I29" s="95"/>
+      <c r="J29" s="95"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="95"/>
+      <c r="M29" s="95"/>
+      <c r="N29" s="95"/>
+      <c r="O29" s="95"/>
+      <c r="P29" s="95"/>
+      <c r="Q29" s="95"/>
+    </row>
+    <row r="30" spans="1:54" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:54" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="32" spans="1:54" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="33" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="34" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="35" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="36" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="37" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="38" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="39" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="40" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="41" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="42" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="43" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="44" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="45" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="46" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="47" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="48" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="49" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="50" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="51" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="52" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="53" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="54" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="55" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="56" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="57" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="58" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="59" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="60" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="61" s="77" customFormat="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A25:Q25"/>
+    <mergeCell ref="A26:Q26"/>
+    <mergeCell ref="A27:Q27"/>
+    <mergeCell ref="A28:Q28"/>
+    <mergeCell ref="A29:Q29"/>
     <mergeCell ref="A24:Q24"/>
     <mergeCell ref="A1:AB1"/>
     <mergeCell ref="AC1:BB1"/>
     <mergeCell ref="A21:Q21"/>
     <mergeCell ref="A22:Q22"/>
     <mergeCell ref="A23:Q23"/>
-    <mergeCell ref="A25:Q25"/>
-    <mergeCell ref="A26:Q26"/>
-    <mergeCell ref="A27:Q27"/>
-    <mergeCell ref="A28:Q28"/>
-    <mergeCell ref="A29:Q29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.1328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="29.86328125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="25.265625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.73046875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.1328125" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="9.1328125" style="3"/>
+    <col min="1" max="1" width="30.08984375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="29.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="25.26953125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.08984375" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.08984375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="9" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
@@ -4502,7 +4613,7 @@
       <c r="D1" s="40"/>
       <c r="E1" s="40"/>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -4519,7 +4630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>13</v>
       </c>
@@ -4539,12 +4650,12 @@
         <v>13.378781688359696</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>59</v>
       </c>
@@ -4559,7 +4670,7 @@
       </c>
       <c r="E6" s="84"/>
     </row>
-    <row r="7" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="86">
         <v>28</v>
       </c>
@@ -4574,13 +4685,13 @@
       </c>
       <c r="E7" s="85"/>
     </row>
-    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="81"/>
       <c r="B8" s="81"/>
       <c r="C8" s="82"/>
       <c r="D8" s="82"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>56</v>
       </c>
@@ -4589,14 +4700,14 @@
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
     </row>
-    <row r="11" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
     </row>
-    <row r="12" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>34</v>
       </c>
@@ -4604,7 +4715,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>36</v>
       </c>
@@ -4612,7 +4723,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="10" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>38</v>
       </c>
@@ -4620,19 +4731,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="22"/>
     </row>
-    <row r="16" spans="1:5" s="10" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="24">
         <v>24</v>
       </c>
       <c r="C16" s="21"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
         <v>21</v>
       </c>
@@ -4641,7 +4752,7 @@
       <c r="D18" s="42"/>
       <c r="E18" s="42"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="41" t="s">
         <v>10</v>
       </c>
@@ -4652,7 +4763,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
         <v>22</v>
       </c>
@@ -4663,7 +4774,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
         <v>24</v>
       </c>
@@ -4674,7 +4785,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
       <c r="B22" s="14" t="s">
         <v>26</v>
@@ -4683,17 +4794,17 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>13</v>
       </c>
@@ -4702,7 +4813,7 @@
       <c r="D26" s="42"/>
       <c r="E26" s="42"/>
     </row>
-    <row r="27" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="41" t="s">
         <v>10</v>
       </c>
@@ -4713,7 +4824,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
         <v>14</v>
       </c>
@@ -4724,7 +4835,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="12" t="s">
         <v>58</v>
       </c>
@@ -4733,7 +4844,7 @@
       <c r="D30" s="42"/>
       <c r="E30" s="42"/>
     </row>
-    <row r="31" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="27" t="s">
         <v>43</v>
       </c>
@@ -4750,7 +4861,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="26">
         <v>1997</v>
       </c>
@@ -4763,7 +4874,7 @@
       <c r="D32" s="10"/>
       <c r="E32" s="10"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="26">
         <v>1998</v>
       </c>
@@ -4782,7 +4893,7 @@
         <v>6.6484424338501588E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="26">
         <v>1999</v>
       </c>
@@ -4801,7 +4912,7 @@
         <v>2.9143636995467476E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="26">
         <v>2000</v>
       </c>
@@ -4820,7 +4931,7 @@
         <v>6.8191523924614153E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="26">
         <v>2001</v>
       </c>
@@ -4839,7 +4950,7 @@
         <v>4.0815360868813244E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="26">
         <v>2002</v>
       </c>
@@ -4858,7 +4969,7 @@
         <v>0.10769048766665149</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="26">
         <v>2003</v>
       </c>
@@ -4877,7 +4988,7 @@
         <v>5.9053805049687755E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="26">
         <v>2004</v>
       </c>
@@ -4896,7 +5007,7 @@
         <v>5.8670234757052138E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="26">
         <v>2005</v>
       </c>
@@ -4915,7 +5026,7 @@
         <v>6.1781753631599455E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="26">
         <v>2006</v>
       </c>
@@ -4934,7 +5045,7 @@
         <v>6.5906687839630079E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="31">
         <v>2007</v>
       </c>
@@ -4953,14 +5064,14 @@
         <v>5.9604038733197397E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>47</v>
       </c>
@@ -4968,7 +5079,7 @@
       <c r="C44" s="9"/>
       <c r="D44" s="9"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="34">
         <f>AVERAGE(E33:E42)</f>
         <v>5.8060812902328285E-2</v>
@@ -4977,13 +5088,13 @@
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
       <c r="D46" s="9"/>
     </row>
-    <row r="47" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="44" t="s">
         <v>48</v>
       </c>
@@ -4991,7 +5102,7 @@
       <c r="C47" s="9"/>
       <c r="D47" s="9"/>
     </row>
-    <row r="48" spans="1:5" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="43">
         <f>1/A45</f>
         <v>17.22332068760786</v>
@@ -5009,23 +5120,65 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F1A2AD-3771-4D0A-B6DC-1FAD62FED203}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{64BCBB0B-FC3B-4EEC-86B1-0E47BF69C645}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.59765625" customWidth="1"/>
+    <col min="1" max="1" width="14.6328125" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="15.59765625" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="95" t="s">
+    <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="87" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="11" t="s">
@@ -5035,7 +5188,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -5048,7 +5201,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -5056,12 +5209,11 @@
         <f>Data!C7</f>
         <v>23</v>
       </c>
-      <c r="C3">
-        <f>Data!A7</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="C3" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -5074,7 +5226,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -5087,7 +5239,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -5100,7 +5252,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -5109,8 +5261,8 @@
         <v>17</v>
       </c>
       <c r="C7">
-        <f>B7</f>
-        <v>17</v>
+        <f>'ARB freight'!D3</f>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New information motivates the change.
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\Current CA EPS update\Transportation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\CalEPS outreach 2022\Updated model Sept 2022\variables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1CE54D-E936-4E1D-BF70-14E5056F61E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D31D89BF-9843-4EFD-A79E-A8D0D0952FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
     <sheet name="NTS 1-20" sheetId="11" r:id="rId2"/>
     <sheet name="Data" sheetId="2" r:id="rId3"/>
-    <sheet name="ARB freight" sheetId="12" r:id="rId4"/>
+    <sheet name="CARB" sheetId="12" r:id="rId4"/>
     <sheet name="AVL" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>Car Avg Lifetime, years (Page 22, Table 7)</t>
   </si>
@@ -65,9 +65,6 @@
     <t>http://www.rita.dot.gov/bts/sites/rita.dot.gov.bts/files/publications/national_transportation_statistics/index.html</t>
   </si>
   <si>
-    <t>Oak Ridge National Laboratory</t>
-  </si>
-  <si>
     <t>Table</t>
   </si>
   <si>
@@ -216,15 +213,6 @@
   </si>
   <si>
     <t>Heavy Truck Avg Lifetime, years (Table 3-14, Row 43)</t>
-  </si>
-  <si>
-    <t>Transportation Energy Data Book Ed. 34</t>
-  </si>
-  <si>
-    <t>Table 3-14, Row 43</t>
-  </si>
-  <si>
-    <t>http://cta.ornl.gov/data/tedb34/Spreadsheets/Table3_14.xls</t>
   </si>
   <si>
     <t>National Transportation Statistics 2015</t>
@@ -364,19 +352,28 @@
     <t>We assume passenger and freight modes are the same for aircraft, rail, and ships.</t>
   </si>
   <si>
-    <t>There are no freight motorbikes in the U.S. EPS, so we arbitrarily set their lifetime equal to passenger motorbikes.</t>
-  </si>
-  <si>
     <t>Vehicle Lifetime (years)</t>
   </si>
   <si>
-    <t xml:space="preserve">CARB states limit on truck life is 25 years. </t>
-  </si>
-  <si>
-    <t>Limit to 25 years based on below.</t>
-  </si>
-  <si>
     <t>https://ww2.arb.ca.gov/sites/default/files/2018-12/181204workgrouppresentation.pdf</t>
+  </si>
+  <si>
+    <t>CARB states 15 - 25 years, e.g. below.</t>
+  </si>
+  <si>
+    <t>Take the midpoint.</t>
+  </si>
+  <si>
+    <t>https://ww2.arb.ca.gov/sites/default/files/barcu/regact/2022/acf22/appg.pdf</t>
+  </si>
+  <si>
+    <t>California Air Resources Board</t>
+  </si>
+  <si>
+    <t>Advanced Clean Trucks Cost</t>
+  </si>
+  <si>
+    <t>Slide 5</t>
   </si>
 </sst>
 </file>
@@ -1664,6 +1661,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>197751</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC11524C-A151-2BE6-D9FA-48E763848BA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7759700" y="1187450"/>
+          <a:ext cx="6458851" cy="3477110"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1988,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2001,15 +2042,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2039,7 +2080,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -2054,7 +2095,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -2064,48 +2105,48 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="10">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="9" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="9" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -2115,22 +2156,22 @@
     </row>
     <row r="27" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.35">
@@ -2140,52 +2181,52 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.35">
@@ -2200,47 +2241,42 @@
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B49" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2275,7 +2311,7 @@
   <sheetData>
     <row r="1" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="89" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="89"/>
@@ -2443,7 +2479,7 @@
     </row>
     <row r="3" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="55" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" s="56">
         <v>11306</v>
@@ -2524,7 +2560,7 @@
         <v>14846</v>
       </c>
       <c r="AB3" s="57" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC3" s="55"/>
       <c r="AD3" s="58"/>
@@ -2555,7 +2591,7 @@
     </row>
     <row r="4" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B4" s="60">
         <v>9443</v>
@@ -2636,7 +2672,7 @@
         <v>7907</v>
       </c>
       <c r="AB4" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC4" s="59"/>
       <c r="AD4" s="62"/>
@@ -2667,7 +2703,7 @@
     </row>
     <row r="5" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B5" s="60">
         <v>0</v>
@@ -2748,7 +2784,7 @@
         <v>1470</v>
       </c>
       <c r="AB5" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC5" s="59"/>
       <c r="AD5" s="62"/>
@@ -2779,7 +2815,7 @@
     </row>
     <row r="6" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="59" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B6" s="60">
         <v>1437</v>
@@ -2860,7 +2896,7 @@
         <v>1577</v>
       </c>
       <c r="AB6" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC6" s="59"/>
       <c r="AD6" s="62"/>
@@ -2891,7 +2927,7 @@
     </row>
     <row r="7" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="59" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B7" s="60">
         <v>242</v>
@@ -2972,7 +3008,7 @@
         <v>571</v>
       </c>
       <c r="AB7" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC7" s="59"/>
       <c r="AD7" s="62"/>
@@ -3003,7 +3039,7 @@
     </row>
     <row r="8" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B8" s="60">
         <v>184</v>
@@ -3084,7 +3120,7 @@
         <v>3321</v>
       </c>
       <c r="AB8" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC8" s="59"/>
       <c r="AD8" s="62"/>
@@ -3115,7 +3151,7 @@
     </row>
     <row r="9" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="64" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="65"/>
       <c r="C9" s="65"/>
@@ -3173,7 +3209,7 @@
     </row>
     <row r="10" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" s="67">
         <f>B4/B$3*100</f>
@@ -3287,7 +3323,7 @@
     </row>
     <row r="11" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B11" s="67">
         <v>0</v>
@@ -3399,7 +3435,7 @@
     </row>
     <row r="12" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="59" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B12" s="69">
         <v>12.7</v>
@@ -3511,7 +3547,7 @@
     </row>
     <row r="13" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="69">
         <v>2.1</v>
@@ -3623,7 +3659,7 @@
     </row>
     <row r="14" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B14" s="69">
         <v>1.6</v>
@@ -3735,7 +3771,7 @@
     </row>
     <row r="15" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="55" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B15" s="70"/>
       <c r="C15" s="70"/>
@@ -3793,7 +3829,7 @@
     </row>
     <row r="16" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B16" s="71">
         <v>20</v>
@@ -3905,7 +3941,7 @@
     </row>
     <row r="17" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B17" s="71">
         <v>14.6</v>
@@ -4017,7 +4053,7 @@
     </row>
     <row r="18" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="59" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B18" s="71">
         <v>16.5</v>
@@ -4129,7 +4165,7 @@
     </row>
     <row r="19" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="59" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B19" s="71">
         <v>14.1</v>
@@ -4241,7 +4277,7 @@
     </row>
     <row r="20" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="73" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B20" s="74">
         <v>13.2</v>
@@ -4353,7 +4389,7 @@
     </row>
     <row r="21" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="91" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B21" s="91"/>
       <c r="C21" s="91"/>
@@ -4393,7 +4429,7 @@
     </row>
     <row r="23" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="92" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
@@ -4414,7 +4450,7 @@
     </row>
     <row r="24" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="88" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B24" s="88"/>
       <c r="C24" s="88"/>
@@ -4435,7 +4471,7 @@
     </row>
     <row r="25" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="88" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B25" s="88"/>
       <c r="C25" s="88"/>
@@ -4456,7 +4492,7 @@
     </row>
     <row r="26" spans="1:54" s="76" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="93" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B26" s="93"/>
       <c r="C26" s="93"/>
@@ -4496,7 +4532,7 @@
     </row>
     <row r="28" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="94" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B28" s="94"/>
       <c r="C28" s="94"/>
@@ -4517,7 +4553,7 @@
     </row>
     <row r="29" spans="1:54" s="76" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="95" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B29" s="95"/>
       <c r="C29" s="95"/>
@@ -4606,7 +4642,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -4621,10 +4657,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>6</v>
@@ -4652,21 +4688,21 @@
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E6" s="84"/>
     </row>
@@ -4693,7 +4729,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="42"/>
@@ -4702,38 +4738,38 @@
     </row>
     <row r="11" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="22"/>
     </row>
@@ -4745,7 +4781,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
@@ -4754,21 +4790,21 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="C19" s="41" t="s">
         <v>11</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="C20" s="10">
         <v>33</v>
@@ -4776,10 +4812,10 @@
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="C21" s="10">
         <v>35</v>
@@ -4788,7 +4824,7 @@
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
       <c r="B22" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="15">
         <v>34</v>
@@ -4796,17 +4832,17 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="42"/>
@@ -4815,21 +4851,21 @@
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="C27" s="41" t="s">
         <v>11</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>14</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>15</v>
       </c>
       <c r="C28" s="15">
         <v>33</v>
@@ -4837,7 +4873,7 @@
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
@@ -4846,19 +4882,19 @@
     </row>
     <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="C31" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="D31" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="37" t="s">
         <v>45</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="37" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5073,7 +5109,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -5096,7 +5132,7 @@
     </row>
     <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -5121,10 +5157,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F1A2AD-3771-4D0A-B6DC-1FAD62FED203}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5132,22 +5168,27 @@
     <col min="1" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L6" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -5166,8 +5207,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5179,18 +5220,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="87" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="78">
         <f>ROUND(Data!E3,0)</f>
@@ -5203,19 +5244,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="45">
         <f>Data!C7</f>
         <v>23</v>
       </c>
       <c r="C3" s="9">
-        <v>25</v>
+        <f>CARB!D3</f>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="45">
         <f>ROUND(Data!A16,0)</f>
@@ -5228,7 +5270,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="78">
         <f>ROUND(Data!C22,0)</f>
@@ -5241,7 +5283,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="78">
         <f>ROUND(Data!C28,0)</f>
@@ -5254,15 +5296,15 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="78">
         <f>ROUND(Data!A48,0)</f>
         <v>17</v>
       </c>
       <c r="C7">
-        <f>'ARB freight'!D3</f>
-        <v>25</v>
+        <f>CARB!D3</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated CA files from chris: bcrbq, pei, fopity, avl, bmresp, socdttinty
</commit_message>
<xml_diff>
--- a/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
+++ b/InputData/trans/AVL/Avg Vehicle Lifetime.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\Current CA EPS update\Transportation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ChrisB\Dropbox (Energy Innovation)\Desktop\CalEPS outreach 2022\Updated model Sept 2022\variables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1CE54D-E936-4E1D-BF70-14E5056F61E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D31D89BF-9843-4EFD-A79E-A8D0D0952FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="9" r:id="rId1"/>
     <sheet name="NTS 1-20" sheetId="11" r:id="rId2"/>
     <sheet name="Data" sheetId="2" r:id="rId3"/>
-    <sheet name="ARB freight" sheetId="12" r:id="rId4"/>
+    <sheet name="CARB" sheetId="12" r:id="rId4"/>
     <sheet name="AVL" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>Car Avg Lifetime, years (Page 22, Table 7)</t>
   </si>
@@ -65,9 +65,6 @@
     <t>http://www.rita.dot.gov/bts/sites/rita.dot.gov.bts/files/publications/national_transportation_statistics/index.html</t>
   </si>
   <si>
-    <t>Oak Ridge National Laboratory</t>
-  </si>
-  <si>
     <t>Table</t>
   </si>
   <si>
@@ -216,15 +213,6 @@
   </si>
   <si>
     <t>Heavy Truck Avg Lifetime, years (Table 3-14, Row 43)</t>
-  </si>
-  <si>
-    <t>Transportation Energy Data Book Ed. 34</t>
-  </si>
-  <si>
-    <t>Table 3-14, Row 43</t>
-  </si>
-  <si>
-    <t>http://cta.ornl.gov/data/tedb34/Spreadsheets/Table3_14.xls</t>
   </si>
   <si>
     <t>National Transportation Statistics 2015</t>
@@ -364,19 +352,28 @@
     <t>We assume passenger and freight modes are the same for aircraft, rail, and ships.</t>
   </si>
   <si>
-    <t>There are no freight motorbikes in the U.S. EPS, so we arbitrarily set their lifetime equal to passenger motorbikes.</t>
-  </si>
-  <si>
     <t>Vehicle Lifetime (years)</t>
   </si>
   <si>
-    <t xml:space="preserve">CARB states limit on truck life is 25 years. </t>
-  </si>
-  <si>
-    <t>Limit to 25 years based on below.</t>
-  </si>
-  <si>
     <t>https://ww2.arb.ca.gov/sites/default/files/2018-12/181204workgrouppresentation.pdf</t>
+  </si>
+  <si>
+    <t>CARB states 15 - 25 years, e.g. below.</t>
+  </si>
+  <si>
+    <t>Take the midpoint.</t>
+  </si>
+  <si>
+    <t>https://ww2.arb.ca.gov/sites/default/files/barcu/regact/2022/acf22/appg.pdf</t>
+  </si>
+  <si>
+    <t>California Air Resources Board</t>
+  </si>
+  <si>
+    <t>Advanced Clean Trucks Cost</t>
+  </si>
+  <si>
+    <t>Slide 5</t>
   </si>
 </sst>
 </file>
@@ -1664,6 +1661,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>197751</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>60810</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC11524C-A151-2BE6-D9FA-48E763848BA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7759700" y="1187450"/>
+          <a:ext cx="6458851" cy="3477110"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1988,10 +2029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2001,15 +2042,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2039,7 +2080,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -2054,7 +2095,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -2064,48 +2105,48 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="9" t="s">
-        <v>9</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="10">
-        <v>2015</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" s="9" t="s">
-        <v>60</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B22" s="9" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
@@ -2115,22 +2156,22 @@
     </row>
     <row r="27" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="9" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="2:2" s="9" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B31" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.35">
@@ -2140,52 +2181,52 @@
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" s="13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" s="13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.35">
@@ -2200,47 +2241,42 @@
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B48" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B49" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2275,7 +2311,7 @@
   <sheetData>
     <row r="1" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="89" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B1" s="89"/>
       <c r="C1" s="89"/>
@@ -2443,7 +2479,7 @@
     </row>
     <row r="3" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="55" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B3" s="56">
         <v>11306</v>
@@ -2524,7 +2560,7 @@
         <v>14846</v>
       </c>
       <c r="AB3" s="57" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC3" s="55"/>
       <c r="AD3" s="58"/>
@@ -2555,7 +2591,7 @@
     </row>
     <row r="4" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B4" s="60">
         <v>9443</v>
@@ -2636,7 +2672,7 @@
         <v>7907</v>
       </c>
       <c r="AB4" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC4" s="59"/>
       <c r="AD4" s="62"/>
@@ -2667,7 +2703,7 @@
     </row>
     <row r="5" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B5" s="60">
         <v>0</v>
@@ -2748,7 +2784,7 @@
         <v>1470</v>
       </c>
       <c r="AB5" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC5" s="59"/>
       <c r="AD5" s="62"/>
@@ -2779,7 +2815,7 @@
     </row>
     <row r="6" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="59" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B6" s="60">
         <v>1437</v>
@@ -2860,7 +2896,7 @@
         <v>1577</v>
       </c>
       <c r="AB6" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC6" s="59"/>
       <c r="AD6" s="62"/>
@@ -2891,7 +2927,7 @@
     </row>
     <row r="7" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="59" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B7" s="60">
         <v>242</v>
@@ -2972,7 +3008,7 @@
         <v>571</v>
       </c>
       <c r="AB7" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC7" s="59"/>
       <c r="AD7" s="62"/>
@@ -3003,7 +3039,7 @@
     </row>
     <row r="8" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B8" s="60">
         <v>184</v>
@@ -3084,7 +3120,7 @@
         <v>3321</v>
       </c>
       <c r="AB8" s="60" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="AC8" s="59"/>
       <c r="AD8" s="62"/>
@@ -3115,7 +3151,7 @@
     </row>
     <row r="9" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="64" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B9" s="65"/>
       <c r="C9" s="65"/>
@@ -3173,7 +3209,7 @@
     </row>
     <row r="10" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" s="67">
         <f>B4/B$3*100</f>
@@ -3287,7 +3323,7 @@
     </row>
     <row r="11" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B11" s="67">
         <v>0</v>
@@ -3399,7 +3435,7 @@
     </row>
     <row r="12" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="59" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B12" s="69">
         <v>12.7</v>
@@ -3511,7 +3547,7 @@
     </row>
     <row r="13" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="59" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="69">
         <v>2.1</v>
@@ -3623,7 +3659,7 @@
     </row>
     <row r="14" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="59" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B14" s="69">
         <v>1.6</v>
@@ -3735,7 +3771,7 @@
     </row>
     <row r="15" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="55" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B15" s="70"/>
       <c r="C15" s="70"/>
@@ -3793,7 +3829,7 @@
     </row>
     <row r="16" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="59" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B16" s="71">
         <v>20</v>
@@ -3905,7 +3941,7 @@
     </row>
     <row r="17" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="59" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B17" s="71">
         <v>14.6</v>
@@ -4017,7 +4053,7 @@
     </row>
     <row r="18" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="59" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B18" s="71">
         <v>16.5</v>
@@ -4129,7 +4165,7 @@
     </row>
     <row r="19" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="59" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B19" s="71">
         <v>14.1</v>
@@ -4241,7 +4277,7 @@
     </row>
     <row r="20" spans="1:54" s="13" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="73" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B20" s="74">
         <v>13.2</v>
@@ -4353,7 +4389,7 @@
     </row>
     <row r="21" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="91" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B21" s="91"/>
       <c r="C21" s="91"/>
@@ -4393,7 +4429,7 @@
     </row>
     <row r="23" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="92" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B23" s="92"/>
       <c r="C23" s="92"/>
@@ -4414,7 +4450,7 @@
     </row>
     <row r="24" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="88" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B24" s="88"/>
       <c r="C24" s="88"/>
@@ -4435,7 +4471,7 @@
     </row>
     <row r="25" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="88" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B25" s="88"/>
       <c r="C25" s="88"/>
@@ -4456,7 +4492,7 @@
     </row>
     <row r="26" spans="1:54" s="76" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="93" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B26" s="93"/>
       <c r="C26" s="93"/>
@@ -4496,7 +4532,7 @@
     </row>
     <row r="28" spans="1:54" s="76" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="94" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B28" s="94"/>
       <c r="C28" s="94"/>
@@ -4517,7 +4553,7 @@
     </row>
     <row r="29" spans="1:54" s="76" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="95" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B29" s="95"/>
       <c r="C29" s="95"/>
@@ -4606,7 +4642,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
@@ -4621,10 +4657,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>6</v>
@@ -4652,21 +4688,21 @@
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="79" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D6" s="79" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E6" s="84"/>
     </row>
@@ -4693,7 +4729,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="42"/>
       <c r="C10" s="42"/>
@@ -4702,38 +4738,38 @@
     </row>
     <row r="11" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>34</v>
-      </c>
-      <c r="B12" s="19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="19" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="19" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="22"/>
     </row>
@@ -4745,7 +4781,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
@@ -4754,21 +4790,21 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="C19" s="41" t="s">
         <v>11</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="C20" s="10">
         <v>33</v>
@@ -4776,10 +4812,10 @@
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="C21" s="10">
         <v>35</v>
@@ -4788,7 +4824,7 @@
     <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="9"/>
       <c r="B22" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" s="15">
         <v>34</v>
@@ -4796,17 +4832,17 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B26" s="42"/>
       <c r="C26" s="42"/>
@@ -4815,21 +4851,21 @@
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="41" t="s">
+      <c r="C27" s="41" t="s">
         <v>11</v>
-      </c>
-      <c r="C27" s="41" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="16" t="s">
         <v>14</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>15</v>
       </c>
       <c r="C28" s="15">
         <v>33</v>
@@ -4837,7 +4873,7 @@
     </row>
     <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B30" s="42"/>
       <c r="C30" s="42"/>
@@ -4846,19 +4882,19 @@
     </row>
     <row r="31" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="C31" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="D31" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="37" t="s">
         <v>45</v>
-      </c>
-      <c r="D31" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="37" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
@@ -5073,7 +5109,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -5096,7 +5132,7 @@
     </row>
     <row r="47" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
@@ -5121,10 +5157,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4F1A2AD-3771-4D0A-B6DC-1FAD62FED203}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5132,22 +5168,27 @@
     <col min="1" max="16384" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" s="9">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L6" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -5166,8 +5207,8 @@
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5179,18 +5220,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="87" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="78">
         <f>ROUND(Data!E3,0)</f>
@@ -5203,19 +5244,20 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="45">
         <f>Data!C7</f>
         <v>23</v>
       </c>
       <c r="C3" s="9">
-        <v>25</v>
+        <f>CARB!D3</f>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="45">
         <f>ROUND(Data!A16,0)</f>
@@ -5228,7 +5270,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="78">
         <f>ROUND(Data!C22,0)</f>
@@ -5241,7 +5283,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="78">
         <f>ROUND(Data!C28,0)</f>
@@ -5254,15 +5296,15 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="78">
         <f>ROUND(Data!A48,0)</f>
         <v>17</v>
       </c>
       <c r="C7">
-        <f>'ARB freight'!D3</f>
-        <v>25</v>
+        <f>CARB!D3</f>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>